<commit_message>
Keep Table relId unchanged when re-saving
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/AutoFilter/RegularAutoFilter.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/AutoFilter/RegularAutoFilter.xlsx
@@ -112,7 +112,7 @@
 </x:styleSheet>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:A8" totalsRowCount="1">
   <x:autoFilter ref="A1:A7">
     <x:filterColumn colId="0">
@@ -785,7 +785,7 @@
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="1">
-    <x:tablePart r:id="rId12"/>
+    <x:tablePart r:id="rId9"/>
   </x:tableParts>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Fix application of multiple columns with filters Improve loading of custom filters (Still needs work. Needs a good refactoring)
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/AutoFilter/RegularAutoFilter.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/AutoFilter/RegularAutoFilter.xlsx
@@ -13,7 +13,7 @@
     <x:sheet name="Table" sheetId="6" r:id="rId6"/>
   </x:sheets>
   <x:definedNames>
-    <x:definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Single Column Numbers'!$A$1:$A$7</x:definedName>
+    <x:definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Single Column Numbers'!$A$1:$B$8</x:definedName>
     <x:definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Single Column Strings'!$A$1:$A$7</x:definedName>
     <x:definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Single Column Mixed'!$A$1:$A$7</x:definedName>
     <x:definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Multi Column'!$A$1:$C$7</x:definedName>
@@ -23,9 +23,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <x:si>
     <x:t>Numbers</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Names</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jacques</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Alex</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Patrick</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jack</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Neil</x:t>
+  </x:si>
+  <x:si>
+    <x:t>John</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jason</x:t>
   </x:si>
   <x:si>
     <x:t>Strings</x:t>
@@ -418,49 +442,78 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:A7"/>
+  <x:dimension ref="A1:B8"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:1">
+    <x:row r="1" spans="1:2">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:1">
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:2">
       <x:c r="A2" s="0" t="n">
         <x:v>5</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:1" hidden="1">
+      <x:c r="B2" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:2" hidden="1">
       <x:c r="A3" s="0" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:2" hidden="1">
+      <x:c r="A4" s="0" t="n">
         <x:v>4</x:v>
       </x:c>
-    </x:row>
-    <x:row r="4" spans="1:1">
-      <x:c r="A4" s="0" t="n">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:1">
+      <x:c r="B4" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:2">
       <x:c r="A5" s="0" t="n">
         <x:v>3</x:v>
       </x:c>
-    </x:row>
-    <x:row r="6" spans="1:1" hidden="1">
+      <x:c r="B5" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:2" hidden="1">
       <x:c r="A6" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:2" hidden="1">
+      <x:c r="A7" s="0" t="n">
         <x:v>2</x:v>
       </x:c>
-    </x:row>
-    <x:row r="7" spans="1:1">
-      <x:c r="A7" s="0" t="n">
+      <x:c r="B7" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:2">
+      <x:c r="A8" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:A7">
+  <x:autoFilter ref="A1:B8">
     <x:filterColumn colId="0">
       <x:filters>
         <x:filter val="3"/>
@@ -468,8 +521,13 @@
         <x:filter val="5"/>
       </x:filters>
     </x:filterColumn>
-    <x:sortState ref="A2:A7">
-      <x:sortCondition descending="1" ref="A1:A7"/>
+    <x:filterColumn colId="1">
+      <x:customFilters>
+        <x:customFilter val="J*"/>
+      </x:customFilters>
+    </x:filterColumn>
+    <x:sortState ref="A2:B8">
+      <x:sortCondition descending="1" ref="A1:A8"/>
     </x:sortState>
   </x:autoFilter>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
@@ -493,37 +551,37 @@
   <x:sheetData>
     <x:row r="1" spans="1:1">
       <x:c r="A1" s="0" t="s">
-        <x:v>1</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:1">
       <x:c r="A2" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:1" hidden="1">
       <x:c r="A3" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:1">
       <x:c r="A4" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:1">
       <x:c r="A5" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:1" hidden="1">
       <x:c r="A6" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:1">
       <x:c r="A7" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -560,22 +618,22 @@
   <x:sheetData>
     <x:row r="1" spans="1:1">
       <x:c r="A1" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:1">
       <x:c r="A2" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:1">
       <x:c r="A3" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:1" hidden="1">
       <x:c r="A4" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:1" hidden="1">
@@ -628,79 +686,79 @@
   <x:sheetData>
     <x:row r="1" spans="1:3">
       <x:c r="A1" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>1</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:3" hidden="1">
       <x:c r="A2" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B2" s="0" t="n">
         <x:v>5</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:3" hidden="1">
       <x:c r="A3" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B3" s="0" t="n">
         <x:v>4</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:3">
       <x:c r="A4" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B4" s="0" t="n">
         <x:v>3</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:3">
       <x:c r="A5" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B5" s="0" t="n">
         <x:v>3</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:3" hidden="1">
       <x:c r="A6" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B6" s="0" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:3" hidden="1">
       <x:c r="A7" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B7" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>